<commit_message>
Combined ratings and calculated K-alpha for completed routers.
</commit_message>
<xml_diff>
--- a/Milestone_3/Router-Evaluations/CAX30-MG8702-Corey.xlsx
+++ b/Milestone_3/Router-Evaluations/CAX30-MG8702-Corey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Corey\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Corey\CYBR8420-project\Breaking-Down-ISP-Routers-Security-Privacy-Insights\Milestone_3\Router-Evaluations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{882CE886-B85A-448A-9950-288BAFC28E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2966B36A-FC70-406C-A054-FC27F648AF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" activeTab="1" xr2:uid="{E3F8F364-F35B-402B-8CC4-CCB12FF51434}"/>
+    <workbookView xWindow="30720" yWindow="2952" windowWidth="11520" windowHeight="12360" xr2:uid="{E3F8F364-F35B-402B-8CC4-CCB12FF51434}"/>
   </bookViews>
   <sheets>
     <sheet name="CAX30" sheetId="12" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="223">
   <si>
     <t>Security (50%) MODIFIED</t>
   </si>
@@ -708,6 +708,9 @@
   </si>
   <si>
     <t>User sentiment.</t>
+  </si>
+  <si>
+    <t>UG Page 74</t>
   </si>
 </sst>
 </file>
@@ -1043,6 +1046,15 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1061,6 +1073,78 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1075,87 +1159,6 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1496,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{704EBA85-18D3-4BCF-8DC3-95B482E9BA9F}">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView topLeftCell="B74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="C40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52:F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1511,15 +1514,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1545,68 +1548,68 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="29">
         <v>10</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="G3" s="23"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="24"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="25"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="26" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="29">
         <v>10</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="26" t="s">
         <v>181</v>
       </c>
     </row>
@@ -1614,257 +1617,257 @@
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="24"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="25"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="32" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="35">
         <v>5</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="32" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="46"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="22"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="47"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="34"/>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="29">
         <v>10</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="G12" s="40"/>
+      <c r="G12" s="41"/>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="41"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="42"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="43"/>
     </row>
     <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="32" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F15" s="48"/>
-      <c r="G15" s="51"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="52"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="53"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="32" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F18" s="48"/>
-      <c r="G18" s="45"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="46"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="47"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="47"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="26" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="29">
         <v>10</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="F21" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="G21" s="23"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="24"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="25"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="32" t="s">
         <v>84</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="48">
+      <c r="E24" s="35">
         <v>5</v>
       </c>
-      <c r="F24" s="48"/>
-      <c r="G24" s="45" t="s">
+      <c r="F24" s="35"/>
+      <c r="G24" s="32" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1872,525 +1875,529 @@
       <c r="A25" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="46"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="46"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="22"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
       <c r="D27" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="47"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="26" t="s">
         <v>48</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="29">
         <v>7</v>
       </c>
-      <c r="F28" s="56" t="s">
+      <c r="F28" s="45" t="s">
         <v>188</v>
       </c>
-      <c r="G28" s="23"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="24"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="24"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="25"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="26" t="s">
         <v>55</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="29">
         <v>3</v>
       </c>
-      <c r="F32" s="26" t="s">
+      <c r="F32" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="G32" s="23"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="24"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="24"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="25"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="29">
         <v>7</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="G36" s="23"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="24"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="24"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
       <c r="D39" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="25"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23" t="s">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="26" t="s">
         <v>69</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="26">
+      <c r="E40" s="29">
         <v>0</v>
       </c>
-      <c r="F40" s="26" t="s">
+      <c r="F40" s="29" t="s">
         <v>191</v>
       </c>
-      <c r="G40" s="40"/>
+      <c r="G40" s="41"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="43" t="s">
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="41"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="42"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="42"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="43"/>
     </row>
     <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23" t="s">
+      <c r="A43" s="26"/>
+      <c r="B43" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="26" t="s">
         <v>72</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E43" s="26">
+      <c r="E43" s="29">
         <v>10</v>
       </c>
-      <c r="F43" s="26" t="s">
+      <c r="F43" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="G43" s="23" t="s">
+      <c r="G43" s="26" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="24"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
       <c r="D45" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="25"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23" t="s">
+      <c r="A46" s="26"/>
+      <c r="B46" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="32" t="s">
         <v>162</v>
       </c>
       <c r="D46" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="E46" s="48" t="s">
+      <c r="E46" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F46" s="48"/>
-      <c r="G46" s="51"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="38"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="24"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="54" t="s">
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="52"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="53"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="40"/>
     </row>
     <row r="49" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="23" t="s">
+      <c r="A49" s="26"/>
+      <c r="B49" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="26" t="s">
         <v>164</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="40"/>
+      <c r="E49" s="29">
+        <v>10</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="G49" s="41"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="43" t="s">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="41"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="42"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="42"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="43"/>
     </row>
     <row r="52" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="45"/>
-      <c r="B52" s="45" t="s">
+      <c r="A52" s="32"/>
+      <c r="B52" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="45" t="s">
+      <c r="C52" s="32" t="s">
         <v>169</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="E52" s="48" t="s">
+      <c r="E52" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F52" s="48" t="s">
+      <c r="F52" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="G52" s="51"/>
+      <c r="G52" s="38"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="46"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="54" t="s">
+      <c r="A53" s="33"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="E53" s="49"/>
-      <c r="F53" s="49"/>
-      <c r="G53" s="52"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="39"/>
     </row>
     <row r="54" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="47"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="50"/>
-      <c r="G54" s="53"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="40"/>
     </row>
     <row r="55" spans="1:7" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23" t="s">
+      <c r="A55" s="26"/>
+      <c r="B55" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="23" t="s">
+      <c r="C55" s="26" t="s">
         <v>172</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E55" s="26">
+      <c r="E55" s="29">
         <v>10</v>
       </c>
-      <c r="F55" s="26" t="s">
+      <c r="F55" s="29" t="s">
         <v>194</v>
       </c>
-      <c r="G55" s="40"/>
+      <c r="G55" s="41"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="24"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="43" t="s">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="41"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="42"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="25"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="42"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="43"/>
     </row>
     <row r="58" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23" t="s">
+      <c r="A58" s="26"/>
+      <c r="B58" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="26" t="s">
         <v>175</v>
       </c>
       <c r="D58" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E58" s="26">
+      <c r="E58" s="29">
         <v>0</v>
       </c>
-      <c r="F58" s="26"/>
-      <c r="G58" s="40" t="s">
+      <c r="F58" s="29"/>
+      <c r="G58" s="41" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="43" t="s">
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="41"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="42"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="25"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="42"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="43"/>
     </row>
     <row r="61" spans="1:7" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="26" t="s">
         <v>78</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E61" s="26" t="s">
+      <c r="E61" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="F61" s="26"/>
-      <c r="G61" s="40" t="s">
+      <c r="F61" s="29"/>
+      <c r="G61" s="41" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="24"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="41"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="42"/>
     </row>
     <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="24"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
       <c r="D63" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="41"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="42"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="25"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
+      <c r="A64" s="28"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
       <c r="D64" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="42"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="43"/>
     </row>
     <row r="65" spans="1:7" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D65" s="17" t="s">
@@ -2398,105 +2405,105 @@
       </c>
       <c r="E65" s="18">
         <f>SUM(E3:E64)</f>
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="38" t="s">
+      <c r="A66" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B66" s="38"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="25"/>
     </row>
     <row r="67" spans="1:7" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="23" t="s">
+      <c r="A67" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C67" s="23" t="s">
+      <c r="C67" s="26" t="s">
         <v>94</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E67" s="26">
+      <c r="E67" s="29">
         <v>5</v>
       </c>
-      <c r="F67" s="39"/>
-      <c r="G67" s="23"/>
+      <c r="F67" s="52"/>
+      <c r="G67" s="26"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="24"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
       <c r="D68" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="24"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="27"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="25"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
       <c r="D69" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="25"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="28"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B70" s="23" t="s">
+      <c r="B70" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="C70" s="23" t="s">
+      <c r="C70" s="26" t="s">
         <v>98</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E70" s="26">
+      <c r="E70" s="29">
         <v>5</v>
       </c>
-      <c r="F70" s="34" t="s">
+      <c r="F70" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="G70" s="23" t="s">
+      <c r="G70" s="26" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="24"/>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="27"/>
       <c r="D71" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E71" s="27"/>
-      <c r="F71" s="27"/>
-      <c r="G71" s="24"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="30"/>
+      <c r="G71" s="27"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="25"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
+      <c r="A72" s="28"/>
+      <c r="B72" s="28"/>
+      <c r="C72" s="28"/>
       <c r="D72" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="25"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="28"/>
     </row>
     <row r="73" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
@@ -2518,47 +2525,47 @@
       <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B74" s="23" t="s">
+      <c r="B74" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="C74" s="23" t="s">
+      <c r="C74" s="26" t="s">
         <v>108</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E74" s="26">
+      <c r="E74" s="29">
         <v>10</v>
       </c>
-      <c r="F74" s="34" t="s">
+      <c r="F74" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="G74" s="23"/>
+      <c r="G74" s="26"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="24"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="27"/>
       <c r="D75" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="24"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="27"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="25"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
+      <c r="A76" s="28"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="28"/>
       <c r="D76" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="25"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="28"/>
     </row>
     <row r="77" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D77" s="17" t="s">
@@ -2570,200 +2577,200 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="35" t="s">
+      <c r="A78" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="37"/>
+      <c r="B78" s="54"/>
+      <c r="C78" s="54"/>
+      <c r="D78" s="54"/>
+      <c r="E78" s="54"/>
+      <c r="F78" s="54"/>
+      <c r="G78" s="55"/>
     </row>
     <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C79" s="23" t="s">
+      <c r="C79" s="26" t="s">
         <v>116</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E79" s="26">
+      <c r="E79" s="29">
         <v>10</v>
       </c>
-      <c r="F79" s="34" t="s">
+      <c r="F79" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="G79" s="23"/>
+      <c r="G79" s="26"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="24"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="27"/>
       <c r="D80" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="24"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="30"/>
+      <c r="G80" s="27"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="24"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
       <c r="D81" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="24"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="30"/>
+      <c r="G81" s="27"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="25"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
+      <c r="A82" s="28"/>
+      <c r="B82" s="28"/>
+      <c r="C82" s="28"/>
       <c r="D82" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E82" s="28"/>
-      <c r="F82" s="28"/>
-      <c r="G82" s="25"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="28"/>
     </row>
     <row r="83" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B83" s="23" t="s">
+      <c r="B83" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C83" s="23" t="s">
+      <c r="C83" s="26" t="s">
         <v>120</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E83" s="26">
+      <c r="E83" s="29">
         <v>10</v>
       </c>
-      <c r="F83" s="34" t="s">
+      <c r="F83" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="G83" s="23"/>
+      <c r="G83" s="26"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="24"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="27"/>
       <c r="D84" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="24"/>
+      <c r="E84" s="30"/>
+      <c r="F84" s="30"/>
+      <c r="G84" s="27"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="25"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
+      <c r="A85" s="28"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="28"/>
       <c r="D85" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E85" s="28"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="25"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="28"/>
     </row>
     <row r="86" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="23" t="s">
+      <c r="A86" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C86" s="23" t="s">
+      <c r="C86" s="26" t="s">
         <v>161</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E86" s="26">
+      <c r="E86" s="29">
         <v>10</v>
       </c>
-      <c r="F86" s="34" t="s">
+      <c r="F86" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="G86" s="23"/>
+      <c r="G86" s="26"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="24"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
       <c r="D87" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="24"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="27"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="25"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
+      <c r="A88" s="28"/>
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
       <c r="D88" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28"/>
-      <c r="G88" s="25"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="28"/>
     </row>
     <row r="89" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="23" t="s">
+      <c r="A89" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B89" s="23" t="s">
+      <c r="B89" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C89" s="23" t="s">
+      <c r="C89" s="26" t="s">
         <v>131</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E89" s="26">
+      <c r="E89" s="29">
         <v>10</v>
       </c>
-      <c r="F89" s="34" t="s">
+      <c r="F89" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="G89" s="23" t="s">
+      <c r="G89" s="26" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A90" s="24"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="24"/>
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="27"/>
       <c r="D90" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E90" s="32"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="24"/>
+      <c r="E90" s="59"/>
+      <c r="F90" s="30"/>
+      <c r="G90" s="27"/>
     </row>
     <row r="91" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="25"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
+      <c r="A91" s="28"/>
+      <c r="B91" s="28"/>
+      <c r="C91" s="28"/>
       <c r="D91" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E91" s="33"/>
-      <c r="F91" s="28"/>
-      <c r="G91" s="25"/>
+      <c r="E91" s="60"/>
+      <c r="F91" s="31"/>
+      <c r="G91" s="28"/>
     </row>
     <row r="92" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D92" s="17" t="s">
@@ -2775,132 +2782,132 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="29" t="s">
+      <c r="A93" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="B93" s="30"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="30"/>
-      <c r="G93" s="31"/>
+      <c r="B93" s="57"/>
+      <c r="C93" s="57"/>
+      <c r="D93" s="57"/>
+      <c r="E93" s="57"/>
+      <c r="F93" s="57"/>
+      <c r="G93" s="58"/>
     </row>
     <row r="94" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A94" s="23"/>
-      <c r="B94" s="23" t="s">
+      <c r="A94" s="26"/>
+      <c r="B94" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C94" s="23" t="s">
+      <c r="C94" s="26" t="s">
         <v>138</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E94" s="26">
+      <c r="E94" s="29">
         <v>10</v>
       </c>
       <c r="F94" s="13"/>
-      <c r="G94" s="23"/>
+      <c r="G94" s="26"/>
     </row>
     <row r="95" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A95" s="24"/>
-      <c r="B95" s="24"/>
-      <c r="C95" s="24"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="27"/>
       <c r="D95" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E95" s="27"/>
+      <c r="E95" s="30"/>
       <c r="F95" s="14"/>
-      <c r="G95" s="24"/>
+      <c r="G95" s="27"/>
     </row>
     <row r="96" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="25"/>
-      <c r="B96" s="25"/>
-      <c r="C96" s="25"/>
+      <c r="A96" s="28"/>
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
       <c r="D96" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E96" s="28"/>
+      <c r="E96" s="31"/>
       <c r="F96" s="15"/>
-      <c r="G96" s="25"/>
+      <c r="G96" s="28"/>
     </row>
     <row r="97" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A97" s="23"/>
-      <c r="B97" s="23" t="s">
+      <c r="A97" s="26"/>
+      <c r="B97" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C97" s="23" t="s">
+      <c r="C97" s="26" t="s">
         <v>143</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E97" s="26">
+      <c r="E97" s="29">
         <v>10</v>
       </c>
       <c r="F97" s="13"/>
-      <c r="G97" s="23"/>
+      <c r="G97" s="26"/>
     </row>
     <row r="98" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A98" s="24"/>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
       <c r="D98" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E98" s="27"/>
+      <c r="E98" s="30"/>
       <c r="F98" s="14"/>
-      <c r="G98" s="24"/>
+      <c r="G98" s="27"/>
     </row>
     <row r="99" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="25"/>
-      <c r="B99" s="25"/>
-      <c r="C99" s="25"/>
+      <c r="A99" s="28"/>
+      <c r="B99" s="28"/>
+      <c r="C99" s="28"/>
       <c r="D99" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E99" s="28"/>
+      <c r="E99" s="31"/>
       <c r="F99" s="15"/>
-      <c r="G99" s="25"/>
+      <c r="G99" s="28"/>
     </row>
     <row r="100" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A100" s="23"/>
-      <c r="B100" s="23" t="s">
+      <c r="A100" s="26"/>
+      <c r="B100" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="C100" s="23" t="s">
+      <c r="C100" s="26" t="s">
         <v>148</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E100" s="26">
+      <c r="E100" s="29">
         <v>10</v>
       </c>
       <c r="F100" s="13"/>
-      <c r="G100" s="23"/>
+      <c r="G100" s="26"/>
     </row>
     <row r="101" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A101" s="24"/>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
       <c r="D101" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E101" s="27"/>
+      <c r="E101" s="30"/>
       <c r="F101" s="14"/>
-      <c r="G101" s="24"/>
+      <c r="G101" s="27"/>
     </row>
     <row r="102" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="25"/>
-      <c r="B102" s="25"/>
-      <c r="C102" s="25"/>
+      <c r="A102" s="28"/>
+      <c r="B102" s="28"/>
+      <c r="C102" s="28"/>
       <c r="D102" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E102" s="28"/>
+      <c r="E102" s="31"/>
       <c r="F102" s="15"/>
-      <c r="G102" s="25"/>
+      <c r="G102" s="28"/>
     </row>
     <row r="103" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D103" s="17" t="s">
@@ -2930,18 +2937,154 @@
     </row>
   </sheetData>
   <mergeCells count="177">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="E97:E99"/>
+    <mergeCell ref="G97:G99"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="B100:B102"/>
+    <mergeCell ref="C100:C102"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="G100:G102"/>
+    <mergeCell ref="A93:G93"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="E89:E91"/>
+    <mergeCell ref="F89:F91"/>
+    <mergeCell ref="G89:G91"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="G86:G88"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="E83:E85"/>
+    <mergeCell ref="F83:F85"/>
+    <mergeCell ref="G83:G85"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="E79:E82"/>
+    <mergeCell ref="F79:F82"/>
+    <mergeCell ref="G79:G82"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="F74:F76"/>
+    <mergeCell ref="G74:G76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="E70:E72"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="G70:G72"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="E67:E69"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="G67:G69"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="G61:G64"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="F58:F60"/>
+    <mergeCell ref="G58:G60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="G55:G57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="E9:E11"/>
@@ -2959,154 +3102,18 @@
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="F12:F14"/>
     <mergeCell ref="G12:G14"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="F36:F39"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="G32:G35"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="E55:E57"/>
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="G55:G57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="C61:C64"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="G61:G64"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="E58:E60"/>
-    <mergeCell ref="F58:F60"/>
-    <mergeCell ref="G58:G60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="C70:C72"/>
-    <mergeCell ref="E70:E72"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="G70:G72"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="E67:E69"/>
-    <mergeCell ref="F67:F69"/>
-    <mergeCell ref="G67:G69"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="B79:B82"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="E79:E82"/>
-    <mergeCell ref="F79:F82"/>
-    <mergeCell ref="G79:G82"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="F74:F76"/>
-    <mergeCell ref="G74:G76"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="E86:E88"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="G86:G88"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="E83:E85"/>
-    <mergeCell ref="F83:F85"/>
-    <mergeCell ref="G83:G85"/>
-    <mergeCell ref="A93:G93"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="G94:G96"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="E89:E91"/>
-    <mergeCell ref="F89:F91"/>
-    <mergeCell ref="G89:G91"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="B97:B99"/>
-    <mergeCell ref="C97:C99"/>
-    <mergeCell ref="E97:E99"/>
-    <mergeCell ref="G97:G99"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="B100:B102"/>
-    <mergeCell ref="C100:C102"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="G100:G102"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F21" r:id="rId1" xr:uid="{B7A47619-D280-4553-8AFC-973CF9669186}"/>
@@ -3125,7 +3132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DDCBEC-5CAE-4E86-A7AD-6449EAB9F510}">
   <dimension ref="A1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F83" sqref="F83:F85"/>
     </sheetView>
   </sheetViews>
@@ -3140,15 +3147,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -3174,324 +3181,324 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="26" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="29">
         <v>10</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="G3" s="23"/>
+      <c r="G3" s="26"/>
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="24"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="25"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="32" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="45"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="46"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="22"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="47"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="26" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="29">
         <v>10</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="29" t="s">
         <v>218</v>
       </c>
-      <c r="G9" s="23"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="24"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="27"/>
     </row>
     <row r="11" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="25"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="26" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="26">
+      <c r="E12" s="29">
         <v>10</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="40" t="s">
+      <c r="F12" s="29"/>
+      <c r="G12" s="41" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="41"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="42"/>
     </row>
     <row r="14" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="42"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="43"/>
     </row>
     <row r="15" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="32" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F15" s="48"/>
-      <c r="G15" s="51"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="52"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="39"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
+      <c r="A17" s="34"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="53"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="40"/>
     </row>
     <row r="18" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="26" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="29">
         <v>10</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="G18" s="23"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="24"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="25"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="26" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="29">
         <v>10</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="23" t="s">
+      <c r="F21" s="29"/>
+      <c r="G21" s="26" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="24"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="28"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="25"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="26" t="s">
         <v>84</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="48">
+      <c r="E24" s="35">
         <v>7</v>
       </c>
-      <c r="F24" s="48" t="s">
+      <c r="F24" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="G24" s="51" t="s">
+      <c r="G24" s="38" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3499,109 +3506,109 @@
       <c r="A25" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="46"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="46"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
       <c r="D27" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="47"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="34"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="26" t="s">
         <v>48</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="29">
         <v>0</v>
       </c>
-      <c r="F28" s="26"/>
-      <c r="G28" s="23" t="s">
+      <c r="F28" s="29"/>
+      <c r="G28" s="26" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="24"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="24"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="25"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="26" t="s">
         <v>55</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E32" s="29">
         <v>0</v>
       </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="23" t="s">
+      <c r="F32" s="29"/>
+      <c r="G32" s="26" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3609,421 +3616,421 @@
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
       <c r="D33" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="24"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="24"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
       <c r="D35" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="25"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="26" t="s">
         <v>63</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="29">
         <v>10</v>
       </c>
-      <c r="F36" s="26" t="s">
+      <c r="F36" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="G36" s="23"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="24"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="27"/>
     </row>
     <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="24"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="27"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
       <c r="D39" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="25"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23" t="s">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="26" t="s">
         <v>69</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="26">
+      <c r="E40" s="29">
         <v>0</v>
       </c>
-      <c r="F40" s="26"/>
-      <c r="G40" s="40" t="s">
+      <c r="F40" s="29"/>
+      <c r="G40" s="41" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="43" t="s">
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="41"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="42"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="42"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="43"/>
     </row>
     <row r="43" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23" t="s">
+      <c r="A43" s="26"/>
+      <c r="B43" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="26" t="s">
         <v>72</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E43" s="26">
+      <c r="E43" s="29">
         <v>5</v>
       </c>
-      <c r="F43" s="26" t="s">
+      <c r="F43" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="G43" s="23"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="24"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
+      <c r="A45" s="28"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
       <c r="D45" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="25"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="28"/>
     </row>
     <row r="46" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="45"/>
-      <c r="B46" s="45" t="s">
+      <c r="A46" s="32"/>
+      <c r="B46" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="32" t="s">
         <v>162</v>
       </c>
       <c r="D46" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="E46" s="48" t="s">
+      <c r="E46" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F46" s="48"/>
-      <c r="G46" s="51"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="38"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="46"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="54" t="s">
+      <c r="A47" s="33"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="52"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="47"/>
-      <c r="B48" s="47"/>
-      <c r="C48" s="47"/>
-      <c r="D48" s="55"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="53"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="40"/>
     </row>
     <row r="49" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="23" t="s">
+      <c r="A49" s="26"/>
+      <c r="B49" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="26" t="s">
         <v>164</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E49" s="26">
+      <c r="E49" s="29">
         <v>10</v>
       </c>
-      <c r="F49" s="26" t="s">
+      <c r="F49" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="G49" s="40"/>
+      <c r="G49" s="41"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="43" t="s">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="41"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="42"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="44"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="42"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="43"/>
     </row>
     <row r="52" spans="1:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="23"/>
-      <c r="B52" s="23" t="s">
+      <c r="A52" s="26"/>
+      <c r="B52" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="23" t="s">
+      <c r="C52" s="26" t="s">
         <v>169</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="E52" s="26">
+      <c r="E52" s="29">
         <v>10</v>
       </c>
-      <c r="F52" s="26" t="s">
+      <c r="F52" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="G52" s="40"/>
+      <c r="G52" s="41"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="43" t="s">
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="41"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="42"/>
     </row>
     <row r="54" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="44"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="42"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="43"/>
     </row>
     <row r="55" spans="1:7" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23" t="s">
+      <c r="A55" s="26"/>
+      <c r="B55" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="23" t="s">
+      <c r="C55" s="26" t="s">
         <v>172</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E55" s="26">
+      <c r="E55" s="29">
         <v>0</v>
       </c>
-      <c r="F55" s="26"/>
-      <c r="G55" s="40" t="s">
+      <c r="F55" s="29"/>
+      <c r="G55" s="41" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="24"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="43" t="s">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="41"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="42"/>
     </row>
     <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="25"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="42"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="43"/>
     </row>
     <row r="58" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23" t="s">
+      <c r="A58" s="26"/>
+      <c r="B58" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="23" t="s">
+      <c r="C58" s="26" t="s">
         <v>175</v>
       </c>
       <c r="D58" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="E58" s="26">
+      <c r="E58" s="29">
         <v>10</v>
       </c>
-      <c r="F58" s="26" t="s">
+      <c r="F58" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="G58" s="40" t="s">
+      <c r="G58" s="41" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="43" t="s">
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="41"/>
+      <c r="E59" s="30"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="42"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="25"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="42"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="43"/>
     </row>
     <row r="61" spans="1:7" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="23" t="s">
+      <c r="A61" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B61" s="23" t="s">
+      <c r="B61" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="26" t="s">
         <v>78</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E61" s="26">
+      <c r="E61" s="29">
         <v>3</v>
       </c>
-      <c r="F61" s="26" t="s">
+      <c r="F61" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="G61" s="40" t="s">
+      <c r="G61" s="41" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="24"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="41"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="42"/>
     </row>
     <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="24"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
       <c r="D63" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="41"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="42"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="25"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
+      <c r="A64" s="28"/>
+      <c r="B64" s="28"/>
+      <c r="C64" s="28"/>
       <c r="D64" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E64" s="28"/>
-      <c r="F64" s="28"/>
-      <c r="G64" s="42"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="43"/>
     </row>
     <row r="65" spans="1:7" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D65" s="17" t="s">
@@ -4035,97 +4042,97 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="38" t="s">
+      <c r="A66" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B66" s="38"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="25"/>
     </row>
     <row r="67" spans="1:7" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="23" t="s">
+      <c r="A67" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="B67" s="23" t="s">
+      <c r="B67" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C67" s="23" t="s">
+      <c r="C67" s="26" t="s">
         <v>94</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="E67" s="26">
+      <c r="E67" s="29">
         <v>5</v>
       </c>
-      <c r="F67" s="39"/>
-      <c r="G67" s="23"/>
+      <c r="F67" s="52"/>
+      <c r="G67" s="26"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="24"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="27"/>
       <c r="D68" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="24"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="27"/>
     </row>
     <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="25"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
+      <c r="A69" s="28"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
       <c r="D69" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="25"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="28"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="45" t="s">
+      <c r="A70" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="B70" s="45" t="s">
+      <c r="B70" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="C70" s="45" t="s">
+      <c r="C70" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="D70" s="59" t="s">
+      <c r="D70" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="E70" s="48" t="s">
+      <c r="E70" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F70" s="48"/>
-      <c r="G70" s="45"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="32"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="46"/>
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
-      <c r="D71" s="59" t="s">
+      <c r="A71" s="33"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="E71" s="49"/>
-      <c r="F71" s="49"/>
-      <c r="G71" s="46"/>
+      <c r="E71" s="36"/>
+      <c r="F71" s="36"/>
+      <c r="G71" s="33"/>
     </row>
     <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="47"/>
-      <c r="B72" s="47"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="60" t="s">
+      <c r="A72" s="34"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="E72" s="50"/>
-      <c r="F72" s="50"/>
-      <c r="G72" s="47"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="34"/>
     </row>
     <row r="73" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
@@ -4147,49 +4154,49 @@
       <c r="G73" s="2"/>
     </row>
     <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B74" s="23" t="s">
+      <c r="B74" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="C74" s="23" t="s">
+      <c r="C74" s="26" t="s">
         <v>108</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E74" s="26">
+      <c r="E74" s="29">
         <v>5</v>
       </c>
-      <c r="F74" s="34" t="s">
+      <c r="F74" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="G74" s="23" t="s">
+      <c r="G74" s="26" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="24"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="27"/>
       <c r="D75" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="24"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="27"/>
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="25"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
+      <c r="A76" s="28"/>
+      <c r="B76" s="28"/>
+      <c r="C76" s="28"/>
       <c r="D76" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="25"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="28"/>
     </row>
     <row r="77" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D77" s="17" t="s">
@@ -4201,192 +4208,192 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="35" t="s">
+      <c r="A78" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="B78" s="36"/>
-      <c r="C78" s="36"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="36"/>
-      <c r="G78" s="37"/>
+      <c r="B78" s="54"/>
+      <c r="C78" s="54"/>
+      <c r="D78" s="54"/>
+      <c r="E78" s="54"/>
+      <c r="F78" s="54"/>
+      <c r="G78" s="55"/>
     </row>
     <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C79" s="23" t="s">
+      <c r="C79" s="26" t="s">
         <v>116</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E79" s="26">
+      <c r="E79" s="29">
         <v>10</v>
       </c>
-      <c r="F79" s="26"/>
-      <c r="G79" s="23" t="s">
+      <c r="F79" s="29"/>
+      <c r="G79" s="26" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="24"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="27"/>
       <c r="D80" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="24"/>
+      <c r="E80" s="30"/>
+      <c r="F80" s="30"/>
+      <c r="G80" s="27"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A81" s="24"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
       <c r="D81" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="E81" s="27"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="24"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="30"/>
+      <c r="G81" s="27"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="25"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
+      <c r="A82" s="28"/>
+      <c r="B82" s="28"/>
+      <c r="C82" s="28"/>
       <c r="D82" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E82" s="28"/>
-      <c r="F82" s="28"/>
-      <c r="G82" s="25"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="28"/>
     </row>
     <row r="83" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="23" t="s">
+      <c r="A83" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B83" s="23" t="s">
+      <c r="B83" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C83" s="23" t="s">
+      <c r="C83" s="26" t="s">
         <v>120</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E83" s="26">
+      <c r="E83" s="29">
         <v>10</v>
       </c>
-      <c r="F83" s="26"/>
-      <c r="G83" s="23"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="26"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A84" s="24"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="27"/>
       <c r="D84" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E84" s="27"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="24"/>
+      <c r="E84" s="30"/>
+      <c r="F84" s="30"/>
+      <c r="G84" s="27"/>
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="25"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
+      <c r="A85" s="28"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="28"/>
       <c r="D85" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E85" s="28"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="25"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="28"/>
     </row>
     <row r="86" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="23" t="s">
+      <c r="A86" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C86" s="23" t="s">
+      <c r="C86" s="26" t="s">
         <v>161</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E86" s="26">
+      <c r="E86" s="29">
         <v>10</v>
       </c>
-      <c r="F86" s="26"/>
-      <c r="G86" s="23"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="26"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A87" s="24"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
       <c r="D87" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
-      <c r="G87" s="24"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="27"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="25"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
+      <c r="A88" s="28"/>
+      <c r="B88" s="28"/>
+      <c r="C88" s="28"/>
       <c r="D88" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E88" s="28"/>
-      <c r="F88" s="28"/>
-      <c r="G88" s="25"/>
+      <c r="E88" s="31"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="28"/>
     </row>
     <row r="89" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="23" t="s">
+      <c r="A89" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="B89" s="23" t="s">
+      <c r="B89" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C89" s="23" t="s">
+      <c r="C89" s="26" t="s">
         <v>131</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E89" s="26">
+      <c r="E89" s="29">
         <v>10</v>
       </c>
-      <c r="F89" s="26"/>
-      <c r="G89" s="23"/>
+      <c r="F89" s="29"/>
+      <c r="G89" s="26"/>
     </row>
     <row r="90" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A90" s="24"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="24"/>
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="27"/>
       <c r="D90" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E90" s="32"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="24"/>
+      <c r="E90" s="59"/>
+      <c r="F90" s="30"/>
+      <c r="G90" s="27"/>
     </row>
     <row r="91" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="25"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
+      <c r="A91" s="28"/>
+      <c r="B91" s="28"/>
+      <c r="C91" s="28"/>
       <c r="D91" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E91" s="33"/>
-      <c r="F91" s="28"/>
-      <c r="G91" s="25"/>
+      <c r="E91" s="60"/>
+      <c r="F91" s="31"/>
+      <c r="G91" s="28"/>
     </row>
     <row r="92" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D92" s="17" t="s">
@@ -4398,132 +4405,132 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="29" t="s">
+      <c r="A93" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="B93" s="30"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="30"/>
-      <c r="G93" s="31"/>
+      <c r="B93" s="57"/>
+      <c r="C93" s="57"/>
+      <c r="D93" s="57"/>
+      <c r="E93" s="57"/>
+      <c r="F93" s="57"/>
+      <c r="G93" s="58"/>
     </row>
     <row r="94" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A94" s="23"/>
-      <c r="B94" s="23" t="s">
+      <c r="A94" s="26"/>
+      <c r="B94" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C94" s="23" t="s">
+      <c r="C94" s="26" t="s">
         <v>138</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E94" s="26">
+      <c r="E94" s="29">
         <v>10</v>
       </c>
       <c r="F94" s="13"/>
-      <c r="G94" s="23"/>
+      <c r="G94" s="26"/>
     </row>
     <row r="95" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A95" s="24"/>
-      <c r="B95" s="24"/>
-      <c r="C95" s="24"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="27"/>
       <c r="D95" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E95" s="27"/>
+      <c r="E95" s="30"/>
       <c r="F95" s="14"/>
-      <c r="G95" s="24"/>
+      <c r="G95" s="27"/>
     </row>
     <row r="96" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="25"/>
-      <c r="B96" s="25"/>
-      <c r="C96" s="25"/>
+      <c r="A96" s="28"/>
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
       <c r="D96" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E96" s="28"/>
+      <c r="E96" s="31"/>
       <c r="F96" s="15"/>
-      <c r="G96" s="25"/>
+      <c r="G96" s="28"/>
     </row>
     <row r="97" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A97" s="23"/>
-      <c r="B97" s="23" t="s">
+      <c r="A97" s="26"/>
+      <c r="B97" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C97" s="23" t="s">
+      <c r="C97" s="26" t="s">
         <v>143</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E97" s="26">
+      <c r="E97" s="29">
         <v>10</v>
       </c>
       <c r="F97" s="13"/>
-      <c r="G97" s="23"/>
+      <c r="G97" s="26"/>
     </row>
     <row r="98" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A98" s="24"/>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
       <c r="D98" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E98" s="27"/>
+      <c r="E98" s="30"/>
       <c r="F98" s="14"/>
-      <c r="G98" s="24"/>
+      <c r="G98" s="27"/>
     </row>
     <row r="99" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="25"/>
-      <c r="B99" s="25"/>
-      <c r="C99" s="25"/>
+      <c r="A99" s="28"/>
+      <c r="B99" s="28"/>
+      <c r="C99" s="28"/>
       <c r="D99" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E99" s="28"/>
+      <c r="E99" s="31"/>
       <c r="F99" s="15"/>
-      <c r="G99" s="25"/>
+      <c r="G99" s="28"/>
     </row>
     <row r="100" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A100" s="23"/>
-      <c r="B100" s="23" t="s">
+      <c r="A100" s="26"/>
+      <c r="B100" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="C100" s="23" t="s">
+      <c r="C100" s="26" t="s">
         <v>148</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E100" s="26">
+      <c r="E100" s="29">
         <v>10</v>
       </c>
       <c r="F100" s="13"/>
-      <c r="G100" s="23"/>
+      <c r="G100" s="26"/>
     </row>
     <row r="101" spans="1:7" ht="21" x14ac:dyDescent="0.3">
-      <c r="A101" s="24"/>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
       <c r="D101" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E101" s="27"/>
+      <c r="E101" s="30"/>
       <c r="F101" s="14"/>
-      <c r="G101" s="24"/>
+      <c r="G101" s="27"/>
     </row>
     <row r="102" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="25"/>
-      <c r="B102" s="25"/>
-      <c r="C102" s="25"/>
+      <c r="A102" s="28"/>
+      <c r="B102" s="28"/>
+      <c r="C102" s="28"/>
       <c r="D102" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E102" s="28"/>
+      <c r="E102" s="31"/>
       <c r="F102" s="15"/>
-      <c r="G102" s="25"/>
+      <c r="G102" s="28"/>
     </row>
     <row r="103" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D103" s="17" t="s">
@@ -4553,18 +4560,154 @@
     </row>
   </sheetData>
   <mergeCells count="177">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="A97:A99"/>
+    <mergeCell ref="B97:B99"/>
+    <mergeCell ref="C97:C99"/>
+    <mergeCell ref="E97:E99"/>
+    <mergeCell ref="G97:G99"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="B100:B102"/>
+    <mergeCell ref="C100:C102"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="G100:G102"/>
+    <mergeCell ref="A93:G93"/>
+    <mergeCell ref="A94:A96"/>
+    <mergeCell ref="B94:B96"/>
+    <mergeCell ref="C94:C96"/>
+    <mergeCell ref="E94:E96"/>
+    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="C89:C91"/>
+    <mergeCell ref="E89:E91"/>
+    <mergeCell ref="F89:F91"/>
+    <mergeCell ref="G89:G91"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="G86:G88"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="E83:E85"/>
+    <mergeCell ref="F83:F85"/>
+    <mergeCell ref="G83:G85"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="E79:E82"/>
+    <mergeCell ref="F79:F82"/>
+    <mergeCell ref="G79:G82"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="F74:F76"/>
+    <mergeCell ref="G74:G76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="E70:E72"/>
+    <mergeCell ref="F70:F72"/>
+    <mergeCell ref="G70:G72"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="E67:E69"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="G67:G69"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="E61:E64"/>
+    <mergeCell ref="F61:F64"/>
+    <mergeCell ref="G61:G64"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="E58:E60"/>
+    <mergeCell ref="F58:F60"/>
+    <mergeCell ref="G58:G60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="C55:C57"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="G55:G57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="F43:F45"/>
+    <mergeCell ref="G43:G45"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="E9:E11"/>
@@ -4582,154 +4725,18 @@
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="F12:F14"/>
     <mergeCell ref="G12:G14"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="F36:F39"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="G32:G35"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="C55:C57"/>
-    <mergeCell ref="E55:E57"/>
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="G55:G57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="C61:C64"/>
-    <mergeCell ref="E61:E64"/>
-    <mergeCell ref="F61:F64"/>
-    <mergeCell ref="G61:G64"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="E58:E60"/>
-    <mergeCell ref="F58:F60"/>
-    <mergeCell ref="G58:G60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="C70:C72"/>
-    <mergeCell ref="E70:E72"/>
-    <mergeCell ref="F70:F72"/>
-    <mergeCell ref="G70:G72"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="E67:E69"/>
-    <mergeCell ref="F67:F69"/>
-    <mergeCell ref="G67:G69"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="B79:B82"/>
-    <mergeCell ref="C79:C82"/>
-    <mergeCell ref="E79:E82"/>
-    <mergeCell ref="F79:F82"/>
-    <mergeCell ref="G79:G82"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="F74:F76"/>
-    <mergeCell ref="G74:G76"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="C86:C88"/>
-    <mergeCell ref="E86:E88"/>
-    <mergeCell ref="F86:F88"/>
-    <mergeCell ref="G86:G88"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="E83:E85"/>
-    <mergeCell ref="F83:F85"/>
-    <mergeCell ref="G83:G85"/>
-    <mergeCell ref="A93:G93"/>
-    <mergeCell ref="A94:A96"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="C94:C96"/>
-    <mergeCell ref="E94:E96"/>
-    <mergeCell ref="G94:G96"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="C89:C91"/>
-    <mergeCell ref="E89:E91"/>
-    <mergeCell ref="F89:F91"/>
-    <mergeCell ref="G89:G91"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="B97:B99"/>
-    <mergeCell ref="C97:C99"/>
-    <mergeCell ref="E97:E99"/>
-    <mergeCell ref="G97:G99"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="B100:B102"/>
-    <mergeCell ref="C100:C102"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="G100:G102"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="G6:G8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F74" r:id="rId1" xr:uid="{E2455986-6458-41B0-899C-E69334CA6878}"/>

</xml_diff>